<commit_message>
manually added missing TX_PROGDIV_CFG parameter to CSTLP protocol
</commit_message>
<xml_diff>
--- a/examples/EMTF_vu13p_r1/src/protocol_CSTLP.xlsx
+++ b/examples/EMTF_vu13p_r1/src/protocol_CSTLP.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="cstlp_mgt_atts" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1793" uniqueCount="1106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1796" uniqueCount="1109">
   <si>
     <t xml:space="preserve">// path</t>
   </si>
@@ -1916,6 +1916,15 @@
   </si>
   <si>
     <t xml:space="preserve">TX_PROGDIV_RATE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TX_PROGDIV_CFG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ignored by import tcl script, copied manually</t>
   </si>
   <si>
     <t xml:space="preserve">TX_RXDETECT_CFG</t>
@@ -3352,7 +3361,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3374,6 +3383,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -3424,7 +3439,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3445,6 +3460,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3453,7 +3472,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3474,10 +3493,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E687"/>
+  <dimension ref="A1:E688"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="A1 A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A448" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A477" activeCellId="0" sqref="A477"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8247,245 +8266,247 @@
       <c r="A477" s="4" t="s">
         <v>631</v>
       </c>
-      <c r="B477" s="4" t="s">
+      <c r="B477" s="5" t="s">
         <v>632</v>
       </c>
-      <c r="C477" s="0"/>
+      <c r="C477" s="0" t="s">
+        <v>633</v>
+      </c>
       <c r="D477" s="0"/>
     </row>
     <row r="478" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A478" s="4" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="B478" s="4" t="s">
-        <v>105</v>
+        <v>635</v>
       </c>
       <c r="C478" s="0"/>
       <c r="D478" s="0"/>
     </row>
     <row r="479" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A479" s="4" t="s">
-        <v>634</v>
+        <v>636</v>
       </c>
       <c r="B479" s="4" t="s">
-        <v>255</v>
+        <v>105</v>
       </c>
       <c r="C479" s="0"/>
       <c r="D479" s="0"/>
     </row>
     <row r="480" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A480" s="4" t="s">
-        <v>635</v>
+        <v>637</v>
       </c>
       <c r="B480" s="4" t="s">
-        <v>115</v>
+        <v>255</v>
       </c>
       <c r="C480" s="0"/>
       <c r="D480" s="0"/>
     </row>
     <row r="481" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A481" s="4" t="s">
-        <v>636</v>
+        <v>638</v>
       </c>
       <c r="B481" s="4" t="s">
-        <v>592</v>
+        <v>115</v>
       </c>
       <c r="C481" s="0"/>
       <c r="D481" s="0"/>
     </row>
     <row r="482" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A482" s="4" t="s">
-        <v>637</v>
+        <v>639</v>
       </c>
       <c r="B482" s="4" t="s">
-        <v>29</v>
+        <v>592</v>
       </c>
       <c r="C482" s="0"/>
       <c r="D482" s="0"/>
     </row>
     <row r="483" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A483" s="4" t="s">
-        <v>638</v>
+        <v>640</v>
       </c>
       <c r="B483" s="4" t="s">
-        <v>471</v>
+        <v>29</v>
       </c>
       <c r="C483" s="0"/>
       <c r="D483" s="0"/>
     </row>
     <row r="484" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A484" s="4" t="s">
-        <v>639</v>
+        <v>641</v>
       </c>
       <c r="B484" s="4" t="s">
-        <v>640</v>
+        <v>471</v>
       </c>
       <c r="C484" s="0"/>
       <c r="D484" s="0"/>
     </row>
     <row r="485" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A485" s="4" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="B485" s="4" t="s">
-        <v>6</v>
+        <v>643</v>
       </c>
       <c r="C485" s="0"/>
       <c r="D485" s="0"/>
     </row>
     <row r="486" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A486" s="4" t="s">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c r="B486" s="4" t="s">
-        <v>643</v>
+        <v>6</v>
       </c>
       <c r="C486" s="0"/>
       <c r="D486" s="0"/>
     </row>
     <row r="487" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A487" s="4" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="B487" s="4" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="C487" s="0"/>
       <c r="D487" s="0"/>
     </row>
     <row r="488" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A488" s="4" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="B488" s="4" t="s">
-        <v>6</v>
+        <v>648</v>
       </c>
       <c r="C488" s="0"/>
       <c r="D488" s="0"/>
     </row>
     <row r="489" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A489" s="4" t="s">
-        <v>647</v>
+        <v>649</v>
       </c>
       <c r="B489" s="4" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="C489" s="0"/>
       <c r="D489" s="0"/>
     </row>
     <row r="490" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A490" s="4" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="B490" s="4" t="s">
-        <v>649</v>
+        <v>29</v>
       </c>
       <c r="C490" s="0"/>
       <c r="D490" s="0"/>
     </row>
     <row r="491" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A491" s="4" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="B491" s="4" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="C491" s="0"/>
       <c r="D491" s="0"/>
     </row>
     <row r="492" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A492" s="4" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="B492" s="4" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="C492" s="0"/>
       <c r="D492" s="0"/>
     </row>
     <row r="493" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A493" s="4" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="B493" s="4" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="C493" s="0"/>
       <c r="D493" s="0"/>
     </row>
     <row r="494" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A494" s="4" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="B494" s="4" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="C494" s="0"/>
       <c r="D494" s="0"/>
     </row>
     <row r="495" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A495" s="4" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="B495" s="4" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="C495" s="0"/>
       <c r="D495" s="0"/>
     </row>
     <row r="496" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A496" s="4" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="B496" s="4" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="C496" s="0"/>
       <c r="D496" s="0"/>
     </row>
     <row r="497" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A497" s="4" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="B497" s="4" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="C497" s="0"/>
       <c r="D497" s="0"/>
     </row>
     <row r="498" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A498" s="4" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="B498" s="4" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="C498" s="0"/>
       <c r="D498" s="0"/>
     </row>
     <row r="499" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A499" s="4" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="B499" s="4" t="s">
-        <v>29</v>
+        <v>668</v>
       </c>
       <c r="C499" s="0"/>
       <c r="D499" s="0"/>
     </row>
     <row r="500" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A500" s="4" t="s">
-        <v>667</v>
+        <v>669</v>
       </c>
       <c r="B500" s="4" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="C500" s="0"/>
       <c r="D500" s="0"/>
     </row>
     <row r="501" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A501" s="4" t="s">
-        <v>668</v>
+        <v>670</v>
       </c>
       <c r="B501" s="4" t="s">
         <v>6</v>
@@ -8495,67 +8516,67 @@
     </row>
     <row r="502" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A502" s="4" t="s">
-        <v>669</v>
+        <v>671</v>
       </c>
       <c r="B502" s="4" t="s">
-        <v>670</v>
+        <v>6</v>
       </c>
       <c r="C502" s="0"/>
       <c r="D502" s="0"/>
     </row>
     <row r="503" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A503" s="4" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="B503" s="4" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="C503" s="0"/>
       <c r="D503" s="0"/>
     </row>
     <row r="504" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A504" s="4" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="B504" s="4" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="C504" s="0"/>
       <c r="D504" s="0"/>
     </row>
     <row r="505" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A505" s="4" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="B505" s="4" t="s">
-        <v>188</v>
+        <v>677</v>
       </c>
       <c r="C505" s="0"/>
       <c r="D505" s="0"/>
     </row>
     <row r="506" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A506" s="4" t="s">
-        <v>676</v>
+        <v>678</v>
       </c>
       <c r="B506" s="4" t="s">
-        <v>6</v>
+        <v>188</v>
       </c>
       <c r="C506" s="0"/>
       <c r="D506" s="0"/>
     </row>
     <row r="507" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A507" s="4" t="s">
-        <v>677</v>
+        <v>679</v>
       </c>
       <c r="B507" s="4" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="C507" s="0"/>
       <c r="D507" s="0"/>
     </row>
     <row r="508" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A508" s="4" t="s">
-        <v>678</v>
+        <v>680</v>
       </c>
       <c r="B508" s="4" t="s">
         <v>29</v>
@@ -8565,57 +8586,57 @@
     </row>
     <row r="509" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A509" s="4" t="s">
-        <v>679</v>
+        <v>681</v>
       </c>
       <c r="B509" s="4" t="s">
-        <v>426</v>
+        <v>29</v>
       </c>
       <c r="C509" s="0"/>
       <c r="D509" s="0"/>
     </row>
     <row r="510" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A510" s="4" t="s">
-        <v>680</v>
+        <v>682</v>
       </c>
       <c r="B510" s="4" t="s">
-        <v>188</v>
+        <v>426</v>
       </c>
       <c r="C510" s="0"/>
       <c r="D510" s="0"/>
     </row>
     <row r="511" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A511" s="4" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="B511" s="4" t="s">
-        <v>449</v>
+        <v>188</v>
       </c>
       <c r="C511" s="0"/>
       <c r="D511" s="0"/>
     </row>
     <row r="512" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A512" s="4" t="s">
-        <v>682</v>
+        <v>684</v>
       </c>
       <c r="B512" s="4" t="s">
-        <v>683</v>
+        <v>449</v>
       </c>
       <c r="C512" s="0"/>
       <c r="D512" s="0"/>
     </row>
     <row r="513" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A513" s="4" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="B513" s="4" t="s">
-        <v>6</v>
+        <v>686</v>
       </c>
       <c r="C513" s="0"/>
       <c r="D513" s="0"/>
     </row>
     <row r="514" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A514" s="4" t="s">
-        <v>685</v>
+        <v>687</v>
       </c>
       <c r="B514" s="4" t="s">
         <v>6</v>
@@ -8625,21 +8646,17 @@
     </row>
     <row r="515" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A515" s="4" t="s">
-        <v>686</v>
+        <v>688</v>
       </c>
       <c r="B515" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C515" s="0"/>
       <c r="D515" s="0"/>
-      <c r="E515" s="0" t="str">
-        <f aca="false">IF(A515&lt;&gt;A515,"X","")</f>
-        <v/>
-      </c>
     </row>
     <row r="516" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A516" s="4" t="s">
-        <v>687</v>
+        <v>689</v>
       </c>
       <c r="B516" s="4" t="s">
         <v>6</v>
@@ -8653,7 +8670,7 @@
     </row>
     <row r="517" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A517" s="4" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
       <c r="B517" s="4" t="s">
         <v>6</v>
@@ -8667,7 +8684,7 @@
     </row>
     <row r="518" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A518" s="4" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
       <c r="B518" s="4" t="s">
         <v>6</v>
@@ -8681,7 +8698,7 @@
     </row>
     <row r="519" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A519" s="4" t="s">
-        <v>690</v>
+        <v>692</v>
       </c>
       <c r="B519" s="4" t="s">
         <v>6</v>
@@ -8695,7 +8712,7 @@
     </row>
     <row r="520" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A520" s="4" t="s">
-        <v>691</v>
+        <v>693</v>
       </c>
       <c r="B520" s="4" t="s">
         <v>6</v>
@@ -8709,7 +8726,7 @@
     </row>
     <row r="521" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A521" s="4" t="s">
-        <v>692</v>
+        <v>694</v>
       </c>
       <c r="B521" s="4" t="s">
         <v>6</v>
@@ -8723,7 +8740,7 @@
     </row>
     <row r="522" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A522" s="4" t="s">
-        <v>693</v>
+        <v>695</v>
       </c>
       <c r="B522" s="4" t="s">
         <v>6</v>
@@ -8737,7 +8754,7 @@
     </row>
     <row r="523" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A523" s="4" t="s">
-        <v>694</v>
+        <v>696</v>
       </c>
       <c r="B523" s="4" t="s">
         <v>6</v>
@@ -8751,10 +8768,10 @@
     </row>
     <row r="524" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A524" s="4" t="s">
-        <v>695</v>
+        <v>697</v>
       </c>
       <c r="B524" s="4" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="C524" s="0"/>
       <c r="D524" s="0"/>
@@ -8765,10 +8782,10 @@
     </row>
     <row r="525" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A525" s="4" t="s">
-        <v>696</v>
+        <v>698</v>
       </c>
       <c r="B525" s="4" t="s">
-        <v>531</v>
+        <v>29</v>
       </c>
       <c r="C525" s="0"/>
       <c r="D525" s="0"/>
@@ -8779,10 +8796,10 @@
     </row>
     <row r="526" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A526" s="4" t="s">
-        <v>697</v>
+        <v>699</v>
       </c>
       <c r="B526" s="4" t="s">
-        <v>29</v>
+        <v>531</v>
       </c>
       <c r="C526" s="0"/>
       <c r="D526" s="0"/>
@@ -8793,10 +8810,10 @@
     </row>
     <row r="527" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A527" s="4" t="s">
-        <v>698</v>
+        <v>700</v>
       </c>
       <c r="B527" s="4" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="C527" s="0"/>
       <c r="D527" s="0"/>
@@ -8807,7 +8824,7 @@
     </row>
     <row r="528" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A528" s="4" t="s">
-        <v>699</v>
+        <v>701</v>
       </c>
       <c r="B528" s="4" t="s">
         <v>6</v>
@@ -8821,10 +8838,10 @@
     </row>
     <row r="529" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A529" s="4" t="s">
-        <v>700</v>
+        <v>702</v>
       </c>
       <c r="B529" s="4" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C529" s="0"/>
       <c r="D529" s="0"/>
@@ -8835,10 +8852,10 @@
     </row>
     <row r="530" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A530" s="4" t="s">
-        <v>701</v>
+        <v>703</v>
       </c>
       <c r="B530" s="4" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C530" s="0"/>
       <c r="D530" s="0"/>
@@ -8849,10 +8866,10 @@
     </row>
     <row r="531" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A531" s="4" t="s">
-        <v>702</v>
+        <v>704</v>
       </c>
       <c r="B531" s="4" t="s">
-        <v>63</v>
+        <v>6</v>
       </c>
       <c r="C531" s="0"/>
       <c r="D531" s="0"/>
@@ -8863,10 +8880,10 @@
     </row>
     <row r="532" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A532" s="4" t="s">
-        <v>703</v>
+        <v>705</v>
       </c>
       <c r="B532" s="4" t="s">
-        <v>6</v>
+        <v>63</v>
       </c>
       <c r="C532" s="0"/>
       <c r="D532" s="0"/>
@@ -8877,7 +8894,7 @@
     </row>
     <row r="533" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A533" s="4" t="s">
-        <v>704</v>
+        <v>706</v>
       </c>
       <c r="B533" s="4" t="s">
         <v>6</v>
@@ -8891,7 +8908,7 @@
     </row>
     <row r="534" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A534" s="4" t="s">
-        <v>705</v>
+        <v>707</v>
       </c>
       <c r="B534" s="4" t="s">
         <v>6</v>
@@ -8905,7 +8922,7 @@
     </row>
     <row r="535" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A535" s="4" t="s">
-        <v>706</v>
+        <v>708</v>
       </c>
       <c r="B535" s="4" t="s">
         <v>6</v>
@@ -8919,7 +8936,7 @@
     </row>
     <row r="536" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A536" s="4" t="s">
-        <v>707</v>
+        <v>709</v>
       </c>
       <c r="B536" s="4" t="s">
         <v>6</v>
@@ -8933,7 +8950,7 @@
     </row>
     <row r="537" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A537" s="4" t="s">
-        <v>708</v>
+        <v>710</v>
       </c>
       <c r="B537" s="4" t="s">
         <v>6</v>
@@ -8947,7 +8964,7 @@
     </row>
     <row r="538" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A538" s="4" t="s">
-        <v>709</v>
+        <v>711</v>
       </c>
       <c r="B538" s="4" t="s">
         <v>6</v>
@@ -8961,7 +8978,7 @@
     </row>
     <row r="539" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A539" s="4" t="s">
-        <v>710</v>
+        <v>712</v>
       </c>
       <c r="B539" s="4" t="s">
         <v>6</v>
@@ -8975,7 +8992,7 @@
     </row>
     <row r="540" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A540" s="4" t="s">
-        <v>711</v>
+        <v>713</v>
       </c>
       <c r="B540" s="4" t="s">
         <v>6</v>
@@ -8989,7 +9006,7 @@
     </row>
     <row r="541" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A541" s="4" t="s">
-        <v>712</v>
+        <v>714</v>
       </c>
       <c r="B541" s="4" t="s">
         <v>6</v>
@@ -9003,7 +9020,7 @@
     </row>
     <row r="542" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A542" s="4" t="s">
-        <v>713</v>
+        <v>715</v>
       </c>
       <c r="B542" s="4" t="s">
         <v>6</v>
@@ -9017,10 +9034,10 @@
     </row>
     <row r="543" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A543" s="4" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
       <c r="B543" s="4" t="s">
-        <v>63</v>
+        <v>6</v>
       </c>
       <c r="C543" s="0"/>
       <c r="D543" s="0"/>
@@ -9031,10 +9048,10 @@
     </row>
     <row r="544" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A544" s="4" t="s">
-        <v>715</v>
+        <v>717</v>
       </c>
       <c r="B544" s="4" t="s">
-        <v>6</v>
+        <v>63</v>
       </c>
       <c r="C544" s="0"/>
       <c r="D544" s="0"/>
@@ -9045,7 +9062,7 @@
     </row>
     <row r="545" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A545" s="4" t="s">
-        <v>716</v>
+        <v>718</v>
       </c>
       <c r="B545" s="4" t="s">
         <v>6</v>
@@ -9059,7 +9076,7 @@
     </row>
     <row r="546" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A546" s="4" t="s">
-        <v>717</v>
+        <v>719</v>
       </c>
       <c r="B546" s="4" t="s">
         <v>6</v>
@@ -9073,7 +9090,7 @@
     </row>
     <row r="547" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A547" s="4" t="s">
-        <v>718</v>
+        <v>720</v>
       </c>
       <c r="B547" s="4" t="s">
         <v>6</v>
@@ -9087,7 +9104,7 @@
     </row>
     <row r="548" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A548" s="4" t="s">
-        <v>719</v>
+        <v>721</v>
       </c>
       <c r="B548" s="4" t="s">
         <v>6</v>
@@ -9100,20 +9117,24 @@
       </c>
     </row>
     <row r="549" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A549" s="0" t="s">
-        <v>720</v>
-      </c>
-      <c r="B549" s="0" t="s">
+      <c r="A549" s="4" t="s">
+        <v>722</v>
+      </c>
+      <c r="B549" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C549" s="0"/>
       <c r="D549" s="0"/>
+      <c r="E549" s="0" t="str">
+        <f aca="false">IF(A549&lt;&gt;A549,"X","")</f>
+        <v/>
+      </c>
     </row>
     <row r="550" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A550" s="4" t="s">
-        <v>721</v>
-      </c>
-      <c r="B550" s="4" t="s">
+      <c r="A550" s="0" t="s">
+        <v>723</v>
+      </c>
+      <c r="B550" s="0" t="s">
         <v>6</v>
       </c>
       <c r="C550" s="0"/>
@@ -9121,7 +9142,7 @@
     </row>
     <row r="551" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A551" s="4" t="s">
-        <v>722</v>
+        <v>724</v>
       </c>
       <c r="B551" s="4" t="s">
         <v>6</v>
@@ -9131,7 +9152,7 @@
     </row>
     <row r="552" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A552" s="4" t="s">
-        <v>723</v>
+        <v>725</v>
       </c>
       <c r="B552" s="4" t="s">
         <v>6</v>
@@ -9141,27 +9162,27 @@
     </row>
     <row r="553" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A553" s="4" t="s">
-        <v>724</v>
+        <v>726</v>
       </c>
       <c r="B553" s="4" t="s">
-        <v>63</v>
+        <v>6</v>
       </c>
       <c r="C553" s="0"/>
       <c r="D553" s="0"/>
     </row>
     <row r="554" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A554" s="4" t="s">
-        <v>725</v>
+        <v>727</v>
       </c>
       <c r="B554" s="4" t="s">
-        <v>6</v>
+        <v>63</v>
       </c>
       <c r="C554" s="0"/>
       <c r="D554" s="0"/>
     </row>
     <row r="555" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A555" s="4" t="s">
-        <v>726</v>
+        <v>728</v>
       </c>
       <c r="B555" s="4" t="s">
         <v>6</v>
@@ -9171,7 +9192,7 @@
     </row>
     <row r="556" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A556" s="4" t="s">
-        <v>727</v>
+        <v>729</v>
       </c>
       <c r="B556" s="4" t="s">
         <v>6</v>
@@ -9181,7 +9202,7 @@
     </row>
     <row r="557" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A557" s="4" t="s">
-        <v>728</v>
+        <v>730</v>
       </c>
       <c r="B557" s="4" t="s">
         <v>6</v>
@@ -9191,7 +9212,7 @@
     </row>
     <row r="558" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A558" s="4" t="s">
-        <v>729</v>
+        <v>731</v>
       </c>
       <c r="B558" s="4" t="s">
         <v>6</v>
@@ -9201,7 +9222,7 @@
     </row>
     <row r="559" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A559" s="4" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="B559" s="4" t="s">
         <v>6</v>
@@ -9211,27 +9232,27 @@
     </row>
     <row r="560" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A560" s="4" t="s">
-        <v>731</v>
+        <v>733</v>
       </c>
       <c r="B560" s="4" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="C560" s="0"/>
       <c r="D560" s="0"/>
     </row>
     <row r="561" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A561" s="4" t="s">
-        <v>732</v>
+        <v>734</v>
       </c>
       <c r="B561" s="4" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="C561" s="0"/>
       <c r="D561" s="0"/>
     </row>
     <row r="562" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A562" s="4" t="s">
-        <v>733</v>
+        <v>735</v>
       </c>
       <c r="B562" s="4" t="s">
         <v>6</v>
@@ -9241,7 +9262,7 @@
     </row>
     <row r="563" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A563" s="4" t="s">
-        <v>734</v>
+        <v>736</v>
       </c>
       <c r="B563" s="4" t="s">
         <v>6</v>
@@ -9251,7 +9272,7 @@
     </row>
     <row r="564" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A564" s="4" t="s">
-        <v>735</v>
+        <v>737</v>
       </c>
       <c r="B564" s="4" t="s">
         <v>6</v>
@@ -9261,7 +9282,7 @@
     </row>
     <row r="565" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A565" s="4" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="B565" s="4" t="s">
         <v>6</v>
@@ -9271,7 +9292,7 @@
     </row>
     <row r="566" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A566" s="4" t="s">
-        <v>737</v>
+        <v>739</v>
       </c>
       <c r="B566" s="4" t="s">
         <v>6</v>
@@ -9281,37 +9302,37 @@
     </row>
     <row r="567" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A567" s="4" t="s">
-        <v>738</v>
+        <v>740</v>
       </c>
       <c r="B567" s="4" t="s">
-        <v>134</v>
+        <v>6</v>
       </c>
       <c r="C567" s="0"/>
       <c r="D567" s="0"/>
     </row>
     <row r="568" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A568" s="4" t="s">
-        <v>739</v>
+        <v>741</v>
       </c>
       <c r="B568" s="4" t="s">
-        <v>112</v>
+        <v>134</v>
       </c>
       <c r="C568" s="0"/>
       <c r="D568" s="0"/>
     </row>
     <row r="569" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A569" s="4" t="s">
-        <v>740</v>
+        <v>742</v>
       </c>
       <c r="B569" s="4" t="s">
-        <v>6</v>
+        <v>112</v>
       </c>
       <c r="C569" s="0"/>
       <c r="D569" s="0"/>
     </row>
     <row r="570" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A570" s="4" t="s">
-        <v>741</v>
+        <v>743</v>
       </c>
       <c r="B570" s="4" t="s">
         <v>6</v>
@@ -9321,7 +9342,7 @@
     </row>
     <row r="571" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A571" s="4" t="s">
-        <v>742</v>
+        <v>744</v>
       </c>
       <c r="B571" s="4" t="s">
         <v>6</v>
@@ -9331,27 +9352,27 @@
     </row>
     <row r="572" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A572" s="4" t="s">
-        <v>743</v>
+        <v>745</v>
       </c>
       <c r="B572" s="4" t="s">
-        <v>468</v>
+        <v>6</v>
       </c>
       <c r="C572" s="0"/>
       <c r="D572" s="0"/>
     </row>
     <row r="573" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A573" s="4" t="s">
-        <v>744</v>
+        <v>746</v>
       </c>
       <c r="B573" s="4" t="s">
-        <v>6</v>
+        <v>468</v>
       </c>
       <c r="C573" s="0"/>
       <c r="D573" s="0"/>
     </row>
     <row r="574" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A574" s="4" t="s">
-        <v>745</v>
+        <v>747</v>
       </c>
       <c r="B574" s="4" t="s">
         <v>6</v>
@@ -9361,7 +9382,7 @@
     </row>
     <row r="575" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A575" s="4" t="s">
-        <v>746</v>
+        <v>748</v>
       </c>
       <c r="B575" s="4" t="s">
         <v>6</v>
@@ -9371,27 +9392,27 @@
     </row>
     <row r="576" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A576" s="4" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
       <c r="B576" s="4" t="s">
-        <v>748</v>
+        <v>6</v>
       </c>
       <c r="C576" s="0"/>
       <c r="D576" s="0"/>
     </row>
     <row r="577" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A577" s="4" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="B577" s="4" t="s">
-        <v>6</v>
+        <v>751</v>
       </c>
       <c r="C577" s="0"/>
       <c r="D577" s="0"/>
     </row>
     <row r="578" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A578" s="4" t="s">
-        <v>750</v>
+        <v>752</v>
       </c>
       <c r="B578" s="4" t="s">
         <v>6</v>
@@ -9401,7 +9422,7 @@
     </row>
     <row r="579" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A579" s="4" t="s">
-        <v>751</v>
+        <v>753</v>
       </c>
       <c r="B579" s="4" t="s">
         <v>6</v>
@@ -9411,7 +9432,7 @@
     </row>
     <row r="580" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A580" s="4" t="s">
-        <v>752</v>
+        <v>754</v>
       </c>
       <c r="B580" s="4" t="s">
         <v>6</v>
@@ -9421,7 +9442,7 @@
     </row>
     <row r="581" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A581" s="4" t="s">
-        <v>753</v>
+        <v>755</v>
       </c>
       <c r="B581" s="4" t="s">
         <v>6</v>
@@ -9431,7 +9452,7 @@
     </row>
     <row r="582" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A582" s="4" t="s">
-        <v>754</v>
+        <v>756</v>
       </c>
       <c r="B582" s="4" t="s">
         <v>6</v>
@@ -9441,7 +9462,7 @@
     </row>
     <row r="583" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A583" s="4" t="s">
-        <v>755</v>
+        <v>757</v>
       </c>
       <c r="B583" s="4" t="s">
         <v>6</v>
@@ -9451,7 +9472,7 @@
     </row>
     <row r="584" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A584" s="4" t="s">
-        <v>756</v>
+        <v>758</v>
       </c>
       <c r="B584" s="4" t="s">
         <v>6</v>
@@ -9461,7 +9482,7 @@
     </row>
     <row r="585" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A585" s="4" t="s">
-        <v>757</v>
+        <v>759</v>
       </c>
       <c r="B585" s="4" t="s">
         <v>6</v>
@@ -9471,7 +9492,7 @@
     </row>
     <row r="586" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A586" s="4" t="s">
-        <v>758</v>
+        <v>760</v>
       </c>
       <c r="B586" s="4" t="s">
         <v>6</v>
@@ -9481,7 +9502,7 @@
     </row>
     <row r="587" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A587" s="4" t="s">
-        <v>759</v>
+        <v>761</v>
       </c>
       <c r="B587" s="4" t="s">
         <v>6</v>
@@ -9491,7 +9512,7 @@
     </row>
     <row r="588" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A588" s="4" t="s">
-        <v>760</v>
+        <v>762</v>
       </c>
       <c r="B588" s="4" t="s">
         <v>6</v>
@@ -9501,7 +9522,7 @@
     </row>
     <row r="589" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A589" s="4" t="s">
-        <v>761</v>
+        <v>763</v>
       </c>
       <c r="B589" s="4" t="s">
         <v>6</v>
@@ -9511,7 +9532,7 @@
     </row>
     <row r="590" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A590" s="4" t="s">
-        <v>762</v>
+        <v>764</v>
       </c>
       <c r="B590" s="4" t="s">
         <v>6</v>
@@ -9521,7 +9542,7 @@
     </row>
     <row r="591" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A591" s="4" t="s">
-        <v>763</v>
+        <v>765</v>
       </c>
       <c r="B591" s="4" t="s">
         <v>6</v>
@@ -9531,7 +9552,7 @@
     </row>
     <row r="592" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A592" s="4" t="s">
-        <v>764</v>
+        <v>766</v>
       </c>
       <c r="B592" s="4" t="s">
         <v>6</v>
@@ -9541,7 +9562,7 @@
     </row>
     <row r="593" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A593" s="4" t="s">
-        <v>765</v>
+        <v>767</v>
       </c>
       <c r="B593" s="4" t="s">
         <v>6</v>
@@ -9551,7 +9572,7 @@
     </row>
     <row r="594" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A594" s="4" t="s">
-        <v>766</v>
+        <v>768</v>
       </c>
       <c r="B594" s="4" t="s">
         <v>6</v>
@@ -9561,7 +9582,7 @@
     </row>
     <row r="595" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A595" s="4" t="s">
-        <v>767</v>
+        <v>769</v>
       </c>
       <c r="B595" s="4" t="s">
         <v>6</v>
@@ -9571,7 +9592,7 @@
     </row>
     <row r="596" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A596" s="4" t="s">
-        <v>768</v>
+        <v>770</v>
       </c>
       <c r="B596" s="4" t="s">
         <v>6</v>
@@ -9581,7 +9602,7 @@
     </row>
     <row r="597" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A597" s="4" t="s">
-        <v>769</v>
+        <v>771</v>
       </c>
       <c r="B597" s="4" t="s">
         <v>6</v>
@@ -9591,7 +9612,7 @@
     </row>
     <row r="598" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A598" s="4" t="s">
-        <v>770</v>
+        <v>772</v>
       </c>
       <c r="B598" s="4" t="s">
         <v>6</v>
@@ -9601,7 +9622,7 @@
     </row>
     <row r="599" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A599" s="4" t="s">
-        <v>771</v>
+        <v>773</v>
       </c>
       <c r="B599" s="4" t="s">
         <v>6</v>
@@ -9611,7 +9632,7 @@
     </row>
     <row r="600" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A600" s="4" t="s">
-        <v>772</v>
+        <v>774</v>
       </c>
       <c r="B600" s="4" t="s">
         <v>6</v>
@@ -9621,7 +9642,7 @@
     </row>
     <row r="601" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A601" s="4" t="s">
-        <v>773</v>
+        <v>775</v>
       </c>
       <c r="B601" s="4" t="s">
         <v>6</v>
@@ -9631,7 +9652,7 @@
     </row>
     <row r="602" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A602" s="4" t="s">
-        <v>774</v>
+        <v>776</v>
       </c>
       <c r="B602" s="4" t="s">
         <v>6</v>
@@ -9641,7 +9662,7 @@
     </row>
     <row r="603" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A603" s="4" t="s">
-        <v>775</v>
+        <v>777</v>
       </c>
       <c r="B603" s="4" t="s">
         <v>6</v>
@@ -9651,7 +9672,7 @@
     </row>
     <row r="604" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A604" s="4" t="s">
-        <v>776</v>
+        <v>778</v>
       </c>
       <c r="B604" s="4" t="s">
         <v>6</v>
@@ -9661,7 +9682,7 @@
     </row>
     <row r="605" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A605" s="4" t="s">
-        <v>777</v>
+        <v>779</v>
       </c>
       <c r="B605" s="4" t="s">
         <v>6</v>
@@ -9671,7 +9692,7 @@
     </row>
     <row r="606" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A606" s="4" t="s">
-        <v>778</v>
+        <v>780</v>
       </c>
       <c r="B606" s="4" t="s">
         <v>6</v>
@@ -9681,7 +9702,7 @@
     </row>
     <row r="607" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A607" s="4" t="s">
-        <v>779</v>
+        <v>781</v>
       </c>
       <c r="B607" s="4" t="s">
         <v>6</v>
@@ -9691,7 +9712,7 @@
     </row>
     <row r="608" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A608" s="4" t="s">
-        <v>780</v>
+        <v>782</v>
       </c>
       <c r="B608" s="4" t="s">
         <v>6</v>
@@ -9701,7 +9722,7 @@
     </row>
     <row r="609" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A609" s="4" t="s">
-        <v>781</v>
+        <v>783</v>
       </c>
       <c r="B609" s="4" t="s">
         <v>6</v>
@@ -9711,7 +9732,7 @@
     </row>
     <row r="610" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A610" s="4" t="s">
-        <v>782</v>
+        <v>784</v>
       </c>
       <c r="B610" s="4" t="s">
         <v>6</v>
@@ -9721,7 +9742,7 @@
     </row>
     <row r="611" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A611" s="4" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="B611" s="4" t="s">
         <v>6</v>
@@ -9731,7 +9752,7 @@
     </row>
     <row r="612" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A612" s="4" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="B612" s="4" t="s">
         <v>6</v>
@@ -9741,7 +9762,7 @@
     </row>
     <row r="613" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A613" s="4" t="s">
-        <v>785</v>
+        <v>787</v>
       </c>
       <c r="B613" s="4" t="s">
         <v>6</v>
@@ -9751,7 +9772,7 @@
     </row>
     <row r="614" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A614" s="4" t="s">
-        <v>786</v>
+        <v>788</v>
       </c>
       <c r="B614" s="4" t="s">
         <v>6</v>
@@ -9761,7 +9782,7 @@
     </row>
     <row r="615" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A615" s="4" t="s">
-        <v>787</v>
+        <v>789</v>
       </c>
       <c r="B615" s="4" t="s">
         <v>6</v>
@@ -9771,7 +9792,7 @@
     </row>
     <row r="616" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A616" s="4" t="s">
-        <v>788</v>
+        <v>790</v>
       </c>
       <c r="B616" s="4" t="s">
         <v>6</v>
@@ -9781,7 +9802,7 @@
     </row>
     <row r="617" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A617" s="4" t="s">
-        <v>789</v>
+        <v>791</v>
       </c>
       <c r="B617" s="4" t="s">
         <v>6</v>
@@ -9791,37 +9812,37 @@
     </row>
     <row r="618" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A618" s="4" t="s">
-        <v>790</v>
+        <v>792</v>
       </c>
       <c r="B618" s="4" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="C618" s="0"/>
       <c r="D618" s="0"/>
     </row>
     <row r="619" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A619" s="4" t="s">
-        <v>791</v>
+        <v>793</v>
       </c>
       <c r="B619" s="4" t="s">
-        <v>257</v>
+        <v>29</v>
       </c>
       <c r="C619" s="0"/>
       <c r="D619" s="0"/>
     </row>
     <row r="620" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A620" s="4" t="s">
-        <v>792</v>
+        <v>794</v>
       </c>
       <c r="B620" s="4" t="s">
-        <v>6</v>
+        <v>257</v>
       </c>
       <c r="C620" s="0"/>
       <c r="D620" s="0"/>
     </row>
     <row r="621" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A621" s="4" t="s">
-        <v>793</v>
+        <v>795</v>
       </c>
       <c r="B621" s="4" t="s">
         <v>6</v>
@@ -9831,27 +9852,27 @@
     </row>
     <row r="622" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A622" s="4" t="s">
-        <v>794</v>
+        <v>796</v>
       </c>
       <c r="B622" s="4" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="C622" s="0"/>
       <c r="D622" s="0"/>
     </row>
     <row r="623" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A623" s="4" t="s">
-        <v>795</v>
+        <v>797</v>
       </c>
       <c r="B623" s="4" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="C623" s="0"/>
       <c r="D623" s="0"/>
     </row>
     <row r="624" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A624" s="4" t="s">
-        <v>796</v>
+        <v>798</v>
       </c>
       <c r="B624" s="4" t="s">
         <v>6</v>
@@ -9861,7 +9882,7 @@
     </row>
     <row r="625" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A625" s="4" t="s">
-        <v>797</v>
+        <v>799</v>
       </c>
       <c r="B625" s="4" t="s">
         <v>6</v>
@@ -9871,7 +9892,7 @@
     </row>
     <row r="626" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A626" s="4" t="s">
-        <v>798</v>
+        <v>800</v>
       </c>
       <c r="B626" s="4" t="s">
         <v>6</v>
@@ -9881,7 +9902,7 @@
     </row>
     <row r="627" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A627" s="4" t="s">
-        <v>799</v>
+        <v>801</v>
       </c>
       <c r="B627" s="4" t="s">
         <v>6</v>
@@ -9891,7 +9912,7 @@
     </row>
     <row r="628" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A628" s="4" t="s">
-        <v>800</v>
+        <v>802</v>
       </c>
       <c r="B628" s="4" t="s">
         <v>6</v>
@@ -9901,7 +9922,7 @@
     </row>
     <row r="629" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A629" s="4" t="s">
-        <v>801</v>
+        <v>803</v>
       </c>
       <c r="B629" s="4" t="s">
         <v>6</v>
@@ -9911,7 +9932,7 @@
     </row>
     <row r="630" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A630" s="4" t="s">
-        <v>802</v>
+        <v>804</v>
       </c>
       <c r="B630" s="4" t="s">
         <v>6</v>
@@ -9921,7 +9942,7 @@
     </row>
     <row r="631" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A631" s="4" t="s">
-        <v>803</v>
+        <v>805</v>
       </c>
       <c r="B631" s="4" t="s">
         <v>6</v>
@@ -9931,27 +9952,27 @@
     </row>
     <row r="632" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A632" s="4" t="s">
-        <v>804</v>
+        <v>806</v>
       </c>
       <c r="B632" s="4" t="s">
-        <v>115</v>
+        <v>6</v>
       </c>
       <c r="C632" s="0"/>
       <c r="D632" s="0"/>
     </row>
     <row r="633" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A633" s="4" t="s">
-        <v>805</v>
+        <v>807</v>
       </c>
       <c r="B633" s="4" t="s">
-        <v>6</v>
+        <v>115</v>
       </c>
       <c r="C633" s="0"/>
       <c r="D633" s="0"/>
     </row>
     <row r="634" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A634" s="4" t="s">
-        <v>806</v>
+        <v>808</v>
       </c>
       <c r="B634" s="4" t="s">
         <v>6</v>
@@ -9961,7 +9982,7 @@
     </row>
     <row r="635" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A635" s="4" t="s">
-        <v>807</v>
+        <v>809</v>
       </c>
       <c r="B635" s="4" t="s">
         <v>6</v>
@@ -9971,7 +9992,7 @@
     </row>
     <row r="636" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A636" s="4" t="s">
-        <v>808</v>
+        <v>810</v>
       </c>
       <c r="B636" s="4" t="s">
         <v>6</v>
@@ -9981,27 +10002,27 @@
     </row>
     <row r="637" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A637" s="4" t="s">
-        <v>809</v>
+        <v>811</v>
       </c>
       <c r="B637" s="4" t="s">
-        <v>498</v>
+        <v>6</v>
       </c>
       <c r="C637" s="0"/>
       <c r="D637" s="0"/>
     </row>
     <row r="638" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A638" s="4" t="s">
-        <v>810</v>
+        <v>812</v>
       </c>
       <c r="B638" s="4" t="s">
-        <v>6</v>
+        <v>498</v>
       </c>
       <c r="C638" s="0"/>
       <c r="D638" s="0"/>
     </row>
     <row r="639" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A639" s="4" t="s">
-        <v>811</v>
+        <v>813</v>
       </c>
       <c r="B639" s="4" t="s">
         <v>6</v>
@@ -10011,27 +10032,27 @@
     </row>
     <row r="640" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A640" s="4" t="s">
-        <v>812</v>
+        <v>814</v>
       </c>
       <c r="B640" s="4" t="s">
-        <v>257</v>
+        <v>6</v>
       </c>
       <c r="C640" s="0"/>
       <c r="D640" s="0"/>
     </row>
     <row r="641" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A641" s="4" t="s">
-        <v>813</v>
+        <v>815</v>
       </c>
       <c r="B641" s="4" t="s">
-        <v>6</v>
+        <v>257</v>
       </c>
       <c r="C641" s="0"/>
       <c r="D641" s="0"/>
     </row>
     <row r="642" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A642" s="4" t="s">
-        <v>814</v>
+        <v>816</v>
       </c>
       <c r="B642" s="4" t="s">
         <v>6</v>
@@ -10041,27 +10062,27 @@
     </row>
     <row r="643" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A643" s="4" t="s">
-        <v>815</v>
+        <v>817</v>
       </c>
       <c r="B643" s="4" t="s">
-        <v>112</v>
+        <v>6</v>
       </c>
       <c r="C643" s="0"/>
       <c r="D643" s="0"/>
     </row>
     <row r="644" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A644" s="4" t="s">
-        <v>816</v>
+        <v>818</v>
       </c>
       <c r="B644" s="4" t="s">
-        <v>6</v>
+        <v>112</v>
       </c>
       <c r="C644" s="0"/>
       <c r="D644" s="0"/>
     </row>
     <row r="645" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A645" s="4" t="s">
-        <v>817</v>
+        <v>819</v>
       </c>
       <c r="B645" s="4" t="s">
         <v>6</v>
@@ -10071,7 +10092,7 @@
     </row>
     <row r="646" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A646" s="4" t="s">
-        <v>818</v>
+        <v>820</v>
       </c>
       <c r="B646" s="4" t="s">
         <v>6</v>
@@ -10081,27 +10102,27 @@
     </row>
     <row r="647" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A647" s="4" t="s">
-        <v>819</v>
+        <v>821</v>
       </c>
       <c r="B647" s="4" t="s">
-        <v>471</v>
+        <v>6</v>
       </c>
       <c r="C647" s="0"/>
       <c r="D647" s="0"/>
     </row>
     <row r="648" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A648" s="4" t="s">
-        <v>820</v>
+        <v>822</v>
       </c>
       <c r="B648" s="4" t="s">
-        <v>6</v>
+        <v>471</v>
       </c>
       <c r="C648" s="0"/>
       <c r="D648" s="0"/>
     </row>
     <row r="649" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A649" s="4" t="s">
-        <v>821</v>
+        <v>823</v>
       </c>
       <c r="B649" s="4" t="s">
         <v>6</v>
@@ -10111,37 +10132,37 @@
     </row>
     <row r="650" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A650" s="4" t="s">
-        <v>822</v>
+        <v>824</v>
       </c>
       <c r="B650" s="4" t="s">
-        <v>823</v>
+        <v>6</v>
       </c>
       <c r="C650" s="0"/>
       <c r="D650" s="0"/>
     </row>
     <row r="651" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A651" s="4" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="B651" s="4" t="s">
-        <v>569</v>
+        <v>826</v>
       </c>
       <c r="C651" s="0"/>
       <c r="D651" s="0"/>
     </row>
     <row r="652" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A652" s="4" t="s">
-        <v>825</v>
+        <v>827</v>
       </c>
       <c r="B652" s="4" t="s">
-        <v>6</v>
+        <v>569</v>
       </c>
       <c r="C652" s="0"/>
       <c r="D652" s="0"/>
     </row>
     <row r="653" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A653" s="4" t="s">
-        <v>826</v>
+        <v>828</v>
       </c>
       <c r="B653" s="4" t="s">
         <v>6</v>
@@ -10151,7 +10172,7 @@
     </row>
     <row r="654" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A654" s="4" t="s">
-        <v>827</v>
+        <v>829</v>
       </c>
       <c r="B654" s="4" t="s">
         <v>6</v>
@@ -10161,7 +10182,7 @@
     </row>
     <row r="655" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A655" s="4" t="s">
-        <v>828</v>
+        <v>830</v>
       </c>
       <c r="B655" s="4" t="s">
         <v>6</v>
@@ -10171,17 +10192,17 @@
     </row>
     <row r="656" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A656" s="4" t="s">
-        <v>829</v>
+        <v>831</v>
       </c>
       <c r="B656" s="4" t="s">
-        <v>63</v>
+        <v>6</v>
       </c>
       <c r="C656" s="0"/>
       <c r="D656" s="0"/>
     </row>
     <row r="657" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A657" s="4" t="s">
-        <v>830</v>
+        <v>832</v>
       </c>
       <c r="B657" s="4" t="s">
         <v>63</v>
@@ -10191,17 +10212,17 @@
     </row>
     <row r="658" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A658" s="4" t="s">
-        <v>831</v>
+        <v>833</v>
       </c>
       <c r="B658" s="4" t="s">
-        <v>569</v>
+        <v>63</v>
       </c>
       <c r="C658" s="0"/>
       <c r="D658" s="0"/>
     </row>
     <row r="659" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A659" s="4" t="s">
-        <v>832</v>
+        <v>834</v>
       </c>
       <c r="B659" s="4" t="s">
         <v>569</v>
@@ -10211,17 +10232,17 @@
     </row>
     <row r="660" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A660" s="4" t="s">
-        <v>833</v>
+        <v>835</v>
       </c>
       <c r="B660" s="4" t="s">
-        <v>6</v>
+        <v>569</v>
       </c>
       <c r="C660" s="0"/>
       <c r="D660" s="0"/>
     </row>
     <row r="661" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A661" s="4" t="s">
-        <v>834</v>
+        <v>836</v>
       </c>
       <c r="B661" s="4" t="s">
         <v>6</v>
@@ -10231,47 +10252,47 @@
     </row>
     <row r="662" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A662" s="4" t="s">
-        <v>835</v>
+        <v>837</v>
       </c>
       <c r="B662" s="4" t="s">
-        <v>115</v>
+        <v>6</v>
       </c>
       <c r="C662" s="0"/>
       <c r="D662" s="0"/>
     </row>
     <row r="663" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A663" s="4" t="s">
-        <v>836</v>
+        <v>838</v>
       </c>
       <c r="B663" s="4" t="s">
-        <v>6</v>
+        <v>115</v>
       </c>
       <c r="C663" s="0"/>
       <c r="D663" s="0"/>
     </row>
     <row r="664" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A664" s="4" t="s">
-        <v>837</v>
+        <v>839</v>
       </c>
       <c r="B664" s="4" t="s">
-        <v>838</v>
+        <v>6</v>
       </c>
       <c r="C664" s="0"/>
       <c r="D664" s="0"/>
     </row>
     <row r="665" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A665" s="4" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="B665" s="4" t="s">
-        <v>6</v>
+        <v>841</v>
       </c>
       <c r="C665" s="0"/>
       <c r="D665" s="0"/>
     </row>
     <row r="666" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A666" s="4" t="s">
-        <v>840</v>
+        <v>842</v>
       </c>
       <c r="B666" s="4" t="s">
         <v>6</v>
@@ -10281,7 +10302,7 @@
     </row>
     <row r="667" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A667" s="4" t="s">
-        <v>841</v>
+        <v>843</v>
       </c>
       <c r="B667" s="4" t="s">
         <v>6</v>
@@ -10291,7 +10312,7 @@
     </row>
     <row r="668" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A668" s="4" t="s">
-        <v>842</v>
+        <v>844</v>
       </c>
       <c r="B668" s="4" t="s">
         <v>6</v>
@@ -10301,7 +10322,7 @@
     </row>
     <row r="669" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A669" s="4" t="s">
-        <v>843</v>
+        <v>845</v>
       </c>
       <c r="B669" s="4" t="s">
         <v>6</v>
@@ -10311,37 +10332,37 @@
     </row>
     <row r="670" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A670" s="4" t="s">
-        <v>844</v>
+        <v>846</v>
       </c>
       <c r="B670" s="4" t="s">
-        <v>845</v>
+        <v>6</v>
       </c>
       <c r="C670" s="0"/>
       <c r="D670" s="0"/>
     </row>
     <row r="671" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A671" s="4" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="B671" s="4" t="s">
-        <v>112</v>
+        <v>848</v>
       </c>
       <c r="C671" s="0"/>
       <c r="D671" s="0"/>
     </row>
     <row r="672" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A672" s="4" t="s">
-        <v>847</v>
+        <v>849</v>
       </c>
       <c r="B672" s="4" t="s">
-        <v>6</v>
+        <v>112</v>
       </c>
       <c r="C672" s="0"/>
       <c r="D672" s="0"/>
     </row>
     <row r="673" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A673" s="4" t="s">
-        <v>848</v>
+        <v>850</v>
       </c>
       <c r="B673" s="4" t="s">
         <v>6</v>
@@ -10351,7 +10372,7 @@
     </row>
     <row r="674" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A674" s="4" t="s">
-        <v>849</v>
+        <v>851</v>
       </c>
       <c r="B674" s="4" t="s">
         <v>6</v>
@@ -10361,27 +10382,27 @@
     </row>
     <row r="675" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A675" s="4" t="s">
-        <v>850</v>
+        <v>852</v>
       </c>
       <c r="B675" s="4" t="s">
-        <v>851</v>
+        <v>6</v>
       </c>
       <c r="C675" s="0"/>
       <c r="D675" s="0"/>
     </row>
     <row r="676" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A676" s="4" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="B676" s="4" t="s">
-        <v>6</v>
+        <v>854</v>
       </c>
       <c r="C676" s="0"/>
       <c r="D676" s="0"/>
     </row>
     <row r="677" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A677" s="4" t="s">
-        <v>853</v>
+        <v>855</v>
       </c>
       <c r="B677" s="4" t="s">
         <v>6</v>
@@ -10391,7 +10412,7 @@
     </row>
     <row r="678" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A678" s="4" t="s">
-        <v>854</v>
+        <v>856</v>
       </c>
       <c r="B678" s="4" t="s">
         <v>6</v>
@@ -10401,7 +10422,7 @@
     </row>
     <row r="679" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A679" s="4" t="s">
-        <v>855</v>
+        <v>857</v>
       </c>
       <c r="B679" s="4" t="s">
         <v>6</v>
@@ -10411,57 +10432,57 @@
     </row>
     <row r="680" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A680" s="4" t="s">
-        <v>856</v>
+        <v>858</v>
       </c>
       <c r="B680" s="4" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="C680" s="0"/>
       <c r="D680" s="0"/>
     </row>
     <row r="681" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A681" s="4" t="s">
-        <v>857</v>
+        <v>859</v>
       </c>
       <c r="B681" s="4" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="C681" s="0"/>
       <c r="D681" s="0"/>
     </row>
     <row r="682" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A682" s="4" t="s">
-        <v>858</v>
+        <v>860</v>
       </c>
       <c r="B682" s="4" t="s">
-        <v>134</v>
+        <v>6</v>
       </c>
       <c r="C682" s="0"/>
       <c r="D682" s="0"/>
     </row>
     <row r="683" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A683" s="4" t="s">
-        <v>859</v>
+        <v>861</v>
       </c>
       <c r="B683" s="4" t="s">
-        <v>257</v>
+        <v>134</v>
       </c>
       <c r="C683" s="0"/>
       <c r="D683" s="0"/>
     </row>
     <row r="684" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A684" s="4" t="s">
-        <v>860</v>
+        <v>862</v>
       </c>
       <c r="B684" s="4" t="s">
-        <v>6</v>
+        <v>257</v>
       </c>
       <c r="C684" s="0"/>
       <c r="D684" s="0"/>
     </row>
     <row r="685" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A685" s="4" t="s">
-        <v>861</v>
+        <v>863</v>
       </c>
       <c r="B685" s="4" t="s">
         <v>6</v>
@@ -10471,7 +10492,7 @@
     </row>
     <row r="686" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A686" s="4" t="s">
-        <v>862</v>
+        <v>864</v>
       </c>
       <c r="B686" s="4" t="s">
         <v>6</v>
@@ -10481,13 +10502,23 @@
     </row>
     <row r="687" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A687" s="4" t="s">
-        <v>863</v>
+        <v>865</v>
       </c>
       <c r="B687" s="4" t="s">
-        <v>471</v>
+        <v>6</v>
       </c>
       <c r="C687" s="0"/>
       <c r="D687" s="0"/>
+    </row>
+    <row r="688" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A688" s="4" t="s">
+        <v>866</v>
+      </c>
+      <c r="B688" s="4" t="s">
+        <v>471</v>
+      </c>
+      <c r="C688" s="0"/>
+      <c r="D688" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -10527,16 +10558,16 @@
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5"/>
+      <c r="C1" s="6"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>864</v>
-      </c>
-      <c r="C2" s="5"/>
+        <v>867</v>
+      </c>
+      <c r="C2" s="6"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
@@ -10545,11 +10576,11 @@
       <c r="B3" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="C3" s="5"/>
+      <c r="C3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>865</v>
+        <v>868</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>29</v>
@@ -10559,7 +10590,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>866</v>
+        <v>869</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>29</v>
@@ -10569,7 +10600,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>867</v>
+        <v>870</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>6</v>
@@ -10579,7 +10610,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>868</v>
+        <v>871</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>6</v>
@@ -10589,7 +10620,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>869</v>
+        <v>872</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>6</v>
@@ -10599,17 +10630,17 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>870</v>
+        <v>873</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>871</v>
+        <v>874</v>
       </c>
       <c r="C9" s="0"/>
       <c r="D9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>872</v>
+        <v>875</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>63</v>
@@ -10619,7 +10650,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>873</v>
+        <v>876</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>6</v>
@@ -10629,7 +10660,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>874</v>
+        <v>877</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>10</v>
@@ -10639,7 +10670,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>875</v>
+        <v>878</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>10</v>
@@ -10649,27 +10680,27 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>876</v>
+        <v>879</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>877</v>
+        <v>880</v>
       </c>
       <c r="C14" s="0"/>
       <c r="D14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>878</v>
+        <v>881</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>879</v>
+        <v>882</v>
       </c>
       <c r="C15" s="0"/>
       <c r="D15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>880</v>
+        <v>883</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>290</v>
@@ -10679,7 +10710,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>881</v>
+        <v>884</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>10</v>
@@ -10709,7 +10740,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>882</v>
+        <v>885</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>10</v>
@@ -10719,7 +10750,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>883</v>
+        <v>886</v>
       </c>
       <c r="B21" s="0" t="s">
         <v>10</v>
@@ -10822,14 +10853,14 @@
         <v>198</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>884</v>
+        <v>887</v>
       </c>
       <c r="C31" s="0"/>
       <c r="D31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>885</v>
+        <v>888</v>
       </c>
       <c r="B32" s="0" t="s">
         <v>10</v>
@@ -10839,20 +10870,20 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>886</v>
+        <v>889</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>887</v>
+        <v>890</v>
       </c>
       <c r="C33" s="0"/>
       <c r="D33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>888</v>
+        <v>891</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>889</v>
+        <v>892</v>
       </c>
       <c r="C34" s="0"/>
       <c r="D34" s="0"/>
@@ -10899,107 +10930,107 @@
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>890</v>
+        <v>893</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>891</v>
+        <v>894</v>
       </c>
       <c r="C39" s="0"/>
       <c r="D39" s="0"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>892</v>
+        <v>895</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>893</v>
+        <v>896</v>
       </c>
       <c r="C40" s="0"/>
       <c r="D40" s="0"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>894</v>
+        <v>897</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>895</v>
+        <v>898</v>
       </c>
       <c r="C41" s="0"/>
       <c r="D41" s="0"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>896</v>
+        <v>899</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>895</v>
+        <v>898</v>
       </c>
       <c r="C42" s="0"/>
       <c r="D42" s="0"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>897</v>
+        <v>900</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>898</v>
+        <v>901</v>
       </c>
       <c r="C43" s="0"/>
       <c r="D43" s="0"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>899</v>
+        <v>902</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>898</v>
+        <v>901</v>
       </c>
       <c r="C44" s="0"/>
       <c r="D44" s="0"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>900</v>
+        <v>903</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>901</v>
+        <v>904</v>
       </c>
       <c r="C45" s="0"/>
       <c r="D45" s="0"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>902</v>
+        <v>905</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>903</v>
+        <v>906</v>
       </c>
       <c r="C46" s="0"/>
       <c r="D46" s="0"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>904</v>
+        <v>907</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>905</v>
+        <v>908</v>
       </c>
       <c r="C47" s="0"/>
       <c r="D47" s="0"/>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>906</v>
+        <v>909</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>907</v>
+        <v>910</v>
       </c>
       <c r="C48" s="0"/>
       <c r="D48" s="0"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>908</v>
+        <v>911</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>82</v>
@@ -11009,7 +11040,7 @@
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>909</v>
+        <v>912</v>
       </c>
       <c r="B50" s="0" t="n">
         <v>160</v>
@@ -11019,7 +11050,7 @@
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>910</v>
+        <v>913</v>
       </c>
       <c r="B51" s="0" t="s">
         <v>107</v>
@@ -11029,7 +11060,7 @@
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>911</v>
+        <v>914</v>
       </c>
       <c r="B52" s="0" t="s">
         <v>125</v>
@@ -11039,47 +11070,47 @@
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>912</v>
+        <v>915</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>913</v>
+        <v>916</v>
       </c>
       <c r="C53" s="0"/>
       <c r="D53" s="0"/>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>914</v>
+        <v>917</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>913</v>
+        <v>916</v>
       </c>
       <c r="C54" s="0"/>
       <c r="D54" s="0"/>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>915</v>
+        <v>918</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>916</v>
+        <v>919</v>
       </c>
       <c r="C55" s="0"/>
       <c r="D55" s="0"/>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>917</v>
+        <v>920</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>918</v>
+        <v>921</v>
       </c>
       <c r="C56" s="0"/>
       <c r="D56" s="0"/>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>919</v>
+        <v>922</v>
       </c>
       <c r="B57" s="0" t="s">
         <v>6</v>
@@ -11089,7 +11120,7 @@
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>920</v>
+        <v>923</v>
       </c>
       <c r="B58" s="0" t="s">
         <v>29</v>
@@ -11099,7 +11130,7 @@
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>921</v>
+        <v>924</v>
       </c>
       <c r="B59" s="0" t="n">
         <v>1</v>
@@ -11109,7 +11140,7 @@
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>922</v>
+        <v>925</v>
       </c>
       <c r="B60" s="0" t="s">
         <v>10</v>
@@ -11119,7 +11150,7 @@
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>923</v>
+        <v>926</v>
       </c>
       <c r="B61" s="0" t="s">
         <v>10</v>
@@ -11129,7 +11160,7 @@
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>924</v>
+        <v>927</v>
       </c>
       <c r="B62" s="0" t="s">
         <v>10</v>
@@ -11139,77 +11170,77 @@
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>925</v>
+        <v>928</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>926</v>
+        <v>929</v>
       </c>
       <c r="C63" s="0"/>
       <c r="D63" s="0"/>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>927</v>
+        <v>930</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>893</v>
+        <v>896</v>
       </c>
       <c r="C64" s="0"/>
       <c r="D64" s="0"/>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>928</v>
+        <v>931</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>895</v>
+        <v>898</v>
       </c>
       <c r="C65" s="0"/>
       <c r="D65" s="0"/>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>929</v>
+        <v>932</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>895</v>
+        <v>898</v>
       </c>
       <c r="C66" s="0"/>
       <c r="D66" s="0"/>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>930</v>
+        <v>933</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>898</v>
+        <v>901</v>
       </c>
       <c r="C67" s="0"/>
       <c r="D67" s="0"/>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>931</v>
+        <v>934</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>898</v>
+        <v>901</v>
       </c>
       <c r="C68" s="0"/>
       <c r="D68" s="0"/>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>932</v>
+        <v>935</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>901</v>
+        <v>904</v>
       </c>
       <c r="C69" s="0"/>
       <c r="D69" s="0"/>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>933</v>
+        <v>936</v>
       </c>
       <c r="B70" s="0" t="s">
         <v>100</v>
@@ -11219,27 +11250,27 @@
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>934</v>
+        <v>937</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>905</v>
+        <v>908</v>
       </c>
       <c r="C71" s="0"/>
       <c r="D71" s="0"/>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>935</v>
+        <v>938</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>936</v>
+        <v>939</v>
       </c>
       <c r="C72" s="0"/>
       <c r="D72" s="0"/>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>937</v>
+        <v>940</v>
       </c>
       <c r="B73" s="0" t="n">
         <v>66</v>
@@ -11249,7 +11280,7 @@
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>938</v>
+        <v>941</v>
       </c>
       <c r="B74" s="0" t="n">
         <v>80</v>
@@ -11259,7 +11290,7 @@
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>939</v>
+        <v>942</v>
       </c>
       <c r="B75" s="0" t="s">
         <v>107</v>
@@ -11269,7 +11300,7 @@
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>940</v>
+        <v>943</v>
       </c>
       <c r="B76" s="0" t="s">
         <v>125</v>
@@ -11279,47 +11310,47 @@
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>941</v>
+        <v>944</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>913</v>
+        <v>916</v>
       </c>
       <c r="C77" s="0"/>
       <c r="D77" s="0"/>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>942</v>
+        <v>945</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>913</v>
+        <v>916</v>
       </c>
       <c r="C78" s="0"/>
       <c r="D78" s="0"/>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>943</v>
+        <v>946</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>916</v>
+        <v>919</v>
       </c>
       <c r="C79" s="0"/>
       <c r="D79" s="0"/>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>944</v>
+        <v>947</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>945</v>
+        <v>948</v>
       </c>
       <c r="C80" s="0"/>
       <c r="D80" s="0"/>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>946</v>
+        <v>949</v>
       </c>
       <c r="B81" s="0" t="s">
         <v>6</v>
@@ -11329,7 +11360,7 @@
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>947</v>
+        <v>950</v>
       </c>
       <c r="B82" s="0" t="s">
         <v>29</v>
@@ -11339,7 +11370,7 @@
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>948</v>
+        <v>951</v>
       </c>
       <c r="B83" s="0" t="n">
         <v>1</v>
@@ -11349,17 +11380,17 @@
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>949</v>
+        <v>952</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>950</v>
+        <v>953</v>
       </c>
       <c r="C84" s="0"/>
       <c r="D84" s="0"/>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>951</v>
+        <v>954</v>
       </c>
       <c r="B85" s="0" t="s">
         <v>10</v>
@@ -11369,7 +11400,7 @@
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>952</v>
+        <v>955</v>
       </c>
       <c r="B86" s="0" t="s">
         <v>10</v>
@@ -11382,14 +11413,14 @@
         <v>253</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>884</v>
+        <v>887</v>
       </c>
       <c r="C87" s="0"/>
       <c r="D87" s="0"/>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>953</v>
+        <v>956</v>
       </c>
       <c r="B88" s="0" t="s">
         <v>10</v>
@@ -11399,7 +11430,7 @@
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>954</v>
+        <v>957</v>
       </c>
       <c r="B89" s="0" t="s">
         <v>10</v>
@@ -11409,7 +11440,7 @@
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>955</v>
+        <v>958</v>
       </c>
       <c r="B90" s="0" t="s">
         <v>10</v>
@@ -11419,7 +11450,7 @@
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>956</v>
+        <v>959</v>
       </c>
       <c r="B91" s="0" t="s">
         <v>10</v>
@@ -11429,7 +11460,7 @@
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>957</v>
+        <v>960</v>
       </c>
       <c r="B92" s="0" t="s">
         <v>115</v>
@@ -11439,7 +11470,7 @@
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>958</v>
+        <v>961</v>
       </c>
       <c r="B93" s="0" t="s">
         <v>115</v>
@@ -11449,7 +11480,7 @@
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>959</v>
+        <v>962</v>
       </c>
       <c r="B94" s="0" t="s">
         <v>6</v>
@@ -11459,7 +11490,7 @@
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>960</v>
+        <v>963</v>
       </c>
       <c r="B95" s="0" t="s">
         <v>6</v>
@@ -11469,40 +11500,40 @@
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>961</v>
+        <v>964</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>962</v>
+        <v>965</v>
       </c>
       <c r="C96" s="0"/>
       <c r="D96" s="0"/>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>963</v>
+        <v>966</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>964</v>
+        <v>967</v>
       </c>
       <c r="C97" s="0"/>
       <c r="D97" s="0"/>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
+        <v>968</v>
+      </c>
+      <c r="B98" s="0" t="s">
         <v>965</v>
-      </c>
-      <c r="B98" s="0" t="s">
-        <v>962</v>
       </c>
       <c r="C98" s="0"/>
       <c r="D98" s="0"/>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>966</v>
+        <v>969</v>
       </c>
       <c r="B99" s="0" t="s">
-        <v>964</v>
+        <v>967</v>
       </c>
       <c r="C99" s="0"/>
       <c r="D99" s="0"/>
@@ -11531,7 +11562,7 @@
       <c r="A102" s="0" t="s">
         <v>519</v>
       </c>
-      <c r="B102" s="6" t="n">
+      <c r="B102" s="7" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -11543,14 +11574,14 @@
         <v>524</v>
       </c>
       <c r="B103" s="0" t="s">
-        <v>967</v>
+        <v>970</v>
       </c>
       <c r="C103" s="0"/>
       <c r="D103" s="0"/>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>968</v>
+        <v>971</v>
       </c>
       <c r="B104" s="0" t="s">
         <v>10</v>
@@ -11560,7 +11591,7 @@
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>969</v>
+        <v>972</v>
       </c>
       <c r="B105" s="0" t="s">
         <v>10</v>
@@ -11570,7 +11601,7 @@
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>970</v>
+        <v>973</v>
       </c>
       <c r="B106" s="0" t="s">
         <v>10</v>
@@ -11580,7 +11611,7 @@
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>971</v>
+        <v>974</v>
       </c>
       <c r="B107" s="0" t="s">
         <v>10</v>
@@ -11590,7 +11621,7 @@
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>972</v>
+        <v>975</v>
       </c>
       <c r="B108" s="0" t="s">
         <v>10</v>
@@ -11600,17 +11631,17 @@
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>973</v>
+        <v>976</v>
       </c>
       <c r="B109" s="0" t="s">
-        <v>974</v>
+        <v>977</v>
       </c>
       <c r="C109" s="0"/>
       <c r="D109" s="0"/>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>975</v>
+        <v>978</v>
       </c>
       <c r="B110" s="0" t="s">
         <v>10</v>
@@ -11620,7 +11651,7 @@
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>976</v>
+        <v>979</v>
       </c>
       <c r="B111" s="0" t="s">
         <v>29</v>
@@ -11630,7 +11661,7 @@
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>977</v>
+        <v>980</v>
       </c>
       <c r="B112" s="0" t="s">
         <v>29</v>
@@ -11640,7 +11671,7 @@
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>978</v>
+        <v>981</v>
       </c>
       <c r="B113" s="0" t="s">
         <v>29</v>
@@ -11650,7 +11681,7 @@
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>979</v>
+        <v>982</v>
       </c>
       <c r="B114" s="0" t="s">
         <v>29</v>
@@ -11660,17 +11691,17 @@
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="B115" s="0" t="s">
-        <v>981</v>
+        <v>984</v>
       </c>
       <c r="C115" s="0"/>
       <c r="D115" s="0"/>
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>700</v>
+        <v>703</v>
       </c>
       <c r="B116" s="0" t="s">
         <v>63</v>
@@ -11680,7 +11711,7 @@
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>701</v>
+        <v>704</v>
       </c>
       <c r="B117" s="0" t="s">
         <v>6</v>
@@ -11690,7 +11721,7 @@
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>702</v>
+        <v>705</v>
       </c>
       <c r="B118" s="0" t="s">
         <v>63</v>
@@ -11700,7 +11731,7 @@
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>703</v>
+        <v>706</v>
       </c>
       <c r="B119" s="0" t="s">
         <v>6</v>
@@ -11710,7 +11741,7 @@
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>705</v>
+        <v>708</v>
       </c>
       <c r="B120" s="0" t="s">
         <v>6</v>
@@ -11720,7 +11751,7 @@
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>982</v>
+        <v>985</v>
       </c>
       <c r="B121" s="0" t="s">
         <v>6</v>
@@ -11730,7 +11761,7 @@
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>983</v>
+        <v>986</v>
       </c>
       <c r="B122" s="0" t="s">
         <v>6</v>
@@ -11740,7 +11771,7 @@
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>984</v>
+        <v>987</v>
       </c>
       <c r="B123" s="0" t="s">
         <v>6</v>
@@ -11750,7 +11781,7 @@
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>985</v>
+        <v>988</v>
       </c>
       <c r="B124" s="0" t="s">
         <v>6</v>
@@ -11760,7 +11791,7 @@
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>986</v>
+        <v>989</v>
       </c>
       <c r="B125" s="0" t="s">
         <v>6</v>
@@ -11770,7 +11801,7 @@
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>987</v>
+        <v>990</v>
       </c>
       <c r="B126" s="0" t="s">
         <v>6</v>
@@ -11780,7 +11811,7 @@
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>988</v>
+        <v>991</v>
       </c>
       <c r="B127" s="0" t="s">
         <v>6</v>
@@ -11790,7 +11821,7 @@
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>989</v>
+        <v>992</v>
       </c>
       <c r="B128" s="0" t="s">
         <v>6</v>
@@ -11800,7 +11831,7 @@
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>990</v>
+        <v>993</v>
       </c>
       <c r="B129" s="0" t="s">
         <v>6</v>
@@ -11810,7 +11841,7 @@
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>991</v>
+        <v>994</v>
       </c>
       <c r="B130" s="0" t="s">
         <v>6</v>
@@ -11820,7 +11851,7 @@
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>992</v>
+        <v>995</v>
       </c>
       <c r="B131" s="0" t="s">
         <v>6</v>
@@ -11830,7 +11861,7 @@
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>993</v>
+        <v>996</v>
       </c>
       <c r="B132" s="0" t="s">
         <v>6</v>
@@ -11840,7 +11871,7 @@
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>994</v>
+        <v>997</v>
       </c>
       <c r="B133" s="0" t="s">
         <v>6</v>
@@ -11850,7 +11881,7 @@
     </row>
     <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>995</v>
+        <v>998</v>
       </c>
       <c r="B134" s="0" t="s">
         <v>112</v>
@@ -11860,7 +11891,7 @@
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>996</v>
+        <v>999</v>
       </c>
       <c r="B135" s="0" t="s">
         <v>112</v>
@@ -11870,7 +11901,7 @@
     </row>
     <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>997</v>
+        <v>1000</v>
       </c>
       <c r="B136" s="0" t="s">
         <v>569</v>
@@ -11880,7 +11911,7 @@
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>998</v>
+        <v>1001</v>
       </c>
       <c r="B137" s="0" t="s">
         <v>569</v>
@@ -11890,7 +11921,7 @@
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>999</v>
+        <v>1002</v>
       </c>
       <c r="B138" s="0" t="s">
         <v>6</v>
@@ -11900,7 +11931,7 @@
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>1000</v>
+        <v>1003</v>
       </c>
       <c r="B139" s="0" t="s">
         <v>6</v>
@@ -11910,7 +11941,7 @@
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>1001</v>
+        <v>1004</v>
       </c>
       <c r="B140" s="0" t="s">
         <v>569</v>
@@ -11920,7 +11951,7 @@
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>1002</v>
+        <v>1005</v>
       </c>
       <c r="B141" s="0" t="s">
         <v>6</v>
@@ -11930,7 +11961,7 @@
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>1003</v>
+        <v>1006</v>
       </c>
       <c r="B142" s="0" t="s">
         <v>29</v>
@@ -11940,7 +11971,7 @@
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>1004</v>
+        <v>1007</v>
       </c>
       <c r="B143" s="0" t="s">
         <v>6</v>
@@ -11950,7 +11981,7 @@
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>1005</v>
+        <v>1008</v>
       </c>
       <c r="B144" s="0" t="s">
         <v>531</v>
@@ -11960,7 +11991,7 @@
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>1006</v>
+        <v>1009</v>
       </c>
       <c r="B145" s="0" t="s">
         <v>6</v>
@@ -11970,7 +12001,7 @@
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>1007</v>
+        <v>1010</v>
       </c>
       <c r="B146" s="0" t="s">
         <v>6</v>
@@ -11980,7 +12011,7 @@
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>1008</v>
+        <v>1011</v>
       </c>
       <c r="B147" s="0" t="s">
         <v>569</v>
@@ -11990,7 +12021,7 @@
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
-        <v>1009</v>
+        <v>1012</v>
       </c>
       <c r="B148" s="0" t="s">
         <v>6</v>
@@ -12000,7 +12031,7 @@
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>1010</v>
+        <v>1013</v>
       </c>
       <c r="B149" s="0" t="s">
         <v>6</v>
@@ -12010,7 +12041,7 @@
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
-        <v>1011</v>
+        <v>1014</v>
       </c>
       <c r="B150" s="0" t="s">
         <v>29</v>
@@ -12020,7 +12051,7 @@
     </row>
     <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
-        <v>1012</v>
+        <v>1015</v>
       </c>
       <c r="B151" s="0" t="s">
         <v>531</v>
@@ -12030,7 +12061,7 @@
     </row>
     <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
-        <v>1013</v>
+        <v>1016</v>
       </c>
       <c r="B152" s="0" t="s">
         <v>29</v>
@@ -12040,7 +12071,7 @@
     </row>
     <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
-        <v>1014</v>
+        <v>1017</v>
       </c>
       <c r="B153" s="0" t="s">
         <v>569</v>
@@ -12050,7 +12081,7 @@
     </row>
     <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
-        <v>1015</v>
+        <v>1018</v>
       </c>
       <c r="B154" s="0" t="s">
         <v>134</v>
@@ -12060,7 +12091,7 @@
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>1016</v>
+        <v>1019</v>
       </c>
       <c r="B155" s="0" t="s">
         <v>134</v>
@@ -12070,7 +12101,7 @@
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
-        <v>1017</v>
+        <v>1020</v>
       </c>
       <c r="B156" s="0" t="s">
         <v>569</v>
@@ -12080,7 +12111,7 @@
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>1018</v>
+        <v>1021</v>
       </c>
       <c r="B157" s="0" t="s">
         <v>29</v>
@@ -12090,17 +12121,17 @@
     </row>
     <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
-        <v>1019</v>
+        <v>1022</v>
       </c>
       <c r="B158" s="0" t="s">
-        <v>1020</v>
+        <v>1023</v>
       </c>
       <c r="C158" s="0"/>
       <c r="D158" s="0"/>
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>1021</v>
+        <v>1024</v>
       </c>
       <c r="B159" s="0" t="s">
         <v>6</v>
@@ -12110,7 +12141,7 @@
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>1022</v>
+        <v>1025</v>
       </c>
       <c r="B160" s="0" t="s">
         <v>6</v>
@@ -12120,7 +12151,7 @@
     </row>
     <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>1023</v>
+        <v>1026</v>
       </c>
       <c r="B161" s="0" t="s">
         <v>115</v>
@@ -12130,17 +12161,17 @@
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>1024</v>
+        <v>1027</v>
       </c>
       <c r="B162" s="0" t="s">
-        <v>1025</v>
+        <v>1028</v>
       </c>
       <c r="C162" s="0"/>
       <c r="D162" s="0"/>
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
-        <v>1026</v>
+        <v>1029</v>
       </c>
       <c r="B163" s="0" t="s">
         <v>6</v>
@@ -12150,7 +12181,7 @@
     </row>
     <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
-        <v>1027</v>
+        <v>1030</v>
       </c>
       <c r="B164" s="0" t="s">
         <v>6</v>
@@ -12160,7 +12191,7 @@
     </row>
     <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>1028</v>
+        <v>1031</v>
       </c>
       <c r="B165" s="0" t="s">
         <v>115</v>
@@ -12170,7 +12201,7 @@
     </row>
     <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>1029</v>
+        <v>1032</v>
       </c>
       <c r="B166" s="0" t="s">
         <v>6</v>
@@ -12180,7 +12211,7 @@
     </row>
     <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
-        <v>1030</v>
+        <v>1033</v>
       </c>
       <c r="B167" s="0" t="s">
         <v>63</v>
@@ -12190,7 +12221,7 @@
     </row>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
-        <v>1031</v>
+        <v>1034</v>
       </c>
       <c r="B168" s="0" t="s">
         <v>6</v>
@@ -12200,7 +12231,7 @@
     </row>
     <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
-        <v>1032</v>
+        <v>1035</v>
       </c>
       <c r="B169" s="0" t="s">
         <v>6</v>
@@ -12210,7 +12241,7 @@
     </row>
     <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
-        <v>1033</v>
+        <v>1036</v>
       </c>
       <c r="B170" s="0" t="s">
         <v>115</v>
@@ -12220,7 +12251,7 @@
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
-        <v>1034</v>
+        <v>1037</v>
       </c>
       <c r="B171" s="0" t="s">
         <v>115</v>
@@ -12230,7 +12261,7 @@
     </row>
     <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
-        <v>1035</v>
+        <v>1038</v>
       </c>
       <c r="B172" s="0" t="s">
         <v>6</v>
@@ -12240,7 +12271,7 @@
     </row>
     <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
-        <v>1036</v>
+        <v>1039</v>
       </c>
       <c r="B173" s="0" t="s">
         <v>6</v>
@@ -12250,7 +12281,7 @@
     </row>
     <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
-        <v>1037</v>
+        <v>1040</v>
       </c>
       <c r="B174" s="0" t="s">
         <v>6</v>
@@ -12260,7 +12291,7 @@
     </row>
     <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
-        <v>1038</v>
+        <v>1041</v>
       </c>
       <c r="B175" s="0" t="s">
         <v>6</v>
@@ -12270,7 +12301,7 @@
     </row>
     <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
-        <v>1039</v>
+        <v>1042</v>
       </c>
       <c r="B176" s="0" t="s">
         <v>6</v>
@@ -12280,7 +12311,7 @@
     </row>
     <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
-        <v>1040</v>
+        <v>1043</v>
       </c>
       <c r="B177" s="0" t="s">
         <v>264</v>
@@ -12290,7 +12321,7 @@
     </row>
     <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
-        <v>1041</v>
+        <v>1044</v>
       </c>
       <c r="B178" s="0" t="s">
         <v>6</v>
@@ -12300,7 +12331,7 @@
     </row>
     <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
-        <v>1042</v>
+        <v>1045</v>
       </c>
       <c r="B179" s="0" t="s">
         <v>6</v>
@@ -12310,7 +12341,7 @@
     </row>
     <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
-        <v>1043</v>
+        <v>1046</v>
       </c>
       <c r="B180" s="0" t="s">
         <v>6</v>
@@ -12320,7 +12351,7 @@
     </row>
     <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
-        <v>1044</v>
+        <v>1047</v>
       </c>
       <c r="B181" s="0" t="s">
         <v>6</v>
@@ -12346,7 +12377,7 @@
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -12369,7 +12400,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1045</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12382,18 +12413,18 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>1046</v>
+        <v>1049</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>2.55</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>1047</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>1048</v>
+        <v>1051</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>2.55</v>
@@ -12418,7 +12449,7 @@
   <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C29" activeCellId="1" sqref="A1 C29"/>
+      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12430,319 +12461,319 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>1049</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>1050</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>1051</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>1052</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>1053</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>1054</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>1055</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>1056</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>1057</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>1058</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>1059</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>1060</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="3" t="s">
-        <v>696</v>
+        <v>699</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>1061</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="3" t="s">
-        <v>794</v>
+        <v>797</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>1062</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="8" t="s">
         <v>427</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>1063</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C16" s="7" t="s">
-        <v>1064</v>
+      <c r="C16" s="8" t="s">
+        <v>1067</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>1065</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="7" t="s">
-        <v>850</v>
+      <c r="C17" s="8" t="s">
+        <v>853</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>1066</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="7" t="s">
-        <v>1067</v>
+      <c r="C18" s="8" t="s">
+        <v>1070</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>1068</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="8" t="s">
         <v>443</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="8" t="s">
         <v>444</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>1070</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C21" s="7" t="s">
-        <v>1071</v>
+      <c r="C21" s="8" t="s">
+        <v>1074</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>1072</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="7" t="s">
-        <v>1073</v>
+      <c r="B22" s="8" t="s">
+        <v>1076</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C23" s="7" t="s">
-        <v>810</v>
+      <c r="C23" s="8" t="s">
+        <v>813</v>
       </c>
       <c r="D23" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C24" s="7" t="s">
-        <v>803</v>
+      <c r="C24" s="8" t="s">
+        <v>806</v>
       </c>
       <c r="D24" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C25" s="7" t="s">
-        <v>744</v>
+      <c r="C25" s="8" t="s">
+        <v>747</v>
       </c>
       <c r="D25" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C26" s="7" t="s">
+      <c r="C26" s="8" t="s">
         <v>514</v>
       </c>
-      <c r="D26" s="6" t="n">
+      <c r="D26" s="7" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C27" s="7"/>
+      <c r="C27" s="8"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>1074</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C29" s="3" t="s">
-        <v>1075</v>
+        <v>1078</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>1061</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="0" t="s">
-        <v>1076</v>
+        <v>1079</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>1077</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="0" t="s">
-        <v>1078</v>
+        <v>1081</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>1079</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>1080</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
-        <v>1081</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
-        <v>1082</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="0" t="s">
-        <v>1084</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="0" t="s">
-        <v>1085</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="0" t="s">
-        <v>1086</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>1087</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="0" t="s">
-        <v>1088</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="0" t="s">
-        <v>1089</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C44" s="1" t="s">
-        <v>1090</v>
+        <v>1093</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>1091</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C45" s="1" t="s">
-        <v>1092</v>
+        <v>1095</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>1093</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C46" s="1" t="s">
-        <v>1094</v>
+        <v>1097</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>1095</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C47" s="1" t="s">
-        <v>1096</v>
+        <v>1099</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>1097</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C48" s="1" t="s">
-        <v>1098</v>
+        <v>1101</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>1099</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C49" s="1" t="s">
-        <v>1100</v>
+        <v>1103</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>1101</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C50" s="1" t="s">
-        <v>1102</v>
+        <v>1105</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>1103</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C51" s="1" t="s">
-        <v>1104</v>
+        <v>1107</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>